<commit_message>
update as per customer changes
</commit_message>
<xml_diff>
--- a/Requirements/CRs_IDs.xlsx
+++ b/Requirements/CRs_IDs.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4E4FB7-960E-46D9-8B19-6260DB98E52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +25,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>client can easily access his account/s</t>
-  </si>
-  <si>
     <t>perform inter account transactions</t>
   </si>
   <si>
@@ -46,11 +44,6 @@
   </si>
   <si>
     <t>The client can login to the system using a secure login.</t>
-  </si>
-  <si>
-    <t>The client should have direct access to
- his/her different accounts 
-where he can view a history of previous transactions.</t>
   </si>
   <si>
     <t>The client should have the ability to perform transactions 
@@ -112,12 +105,18 @@
   </si>
   <si>
     <t>CRs_4.2</t>
+  </si>
+  <si>
+    <t>client can easily access his account</t>
+  </si>
+  <si>
+    <t>The client should have direct access to his/her only one account where he can view a history of previous transactions.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,9 +222,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -239,9 +235,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -278,6 +271,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -559,184 +558,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" style="13" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="16" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+    </row>
+    <row r="3" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="18" t="s">
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18" t="s">
+    <row r="8" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="19"/>
-    </row>
-    <row r="7" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="18" t="s">
+    <row r="9" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="13" t="s">
+    <row r="10" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C10" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="18" t="s">
+    <row r="11" spans="1:23" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="18" t="s">
+      <c r="B12" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="19"/>
-    </row>
-    <row r="12" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="C12" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="C13" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19"/>
+      <c r="B14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="18" t="s">
+    <row r="15" spans="1:23" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="18"/>
+    </row>
+    <row r="16" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="20"/>
-    </row>
-    <row r="16" spans="1:23" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="C16" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="13" t="s">
+      <c r="C17" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>